<commit_message>
Foram ajustados os casos de usos e os diagramas para simplificar as funcionalidades a serem desenvolvidas nessa primeira etapa
</commit_message>
<xml_diff>
--- a/documentacao/Requisitos_HealthTrack.xlsx
+++ b/documentacao/Requisitos_HealthTrack.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09fcd2ee26dcc9ea/FIAP/Heath-Track/projeto/Documentacao/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09fcd2ee26dcc9ea/FIAP/Heath-Track/projeto/app/documentacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="8_{40D21468-006F-42FC-8450-0DE42002BDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{948D4FE5-958A-4BE3-832B-458B0E189DFA}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="8_{40D21468-006F-42FC-8450-0DE42002BDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1DFF0A8-8505-4AAA-9AEA-9A70ECBA43A8}"/>
   <bookViews>
-    <workbookView xWindow="7305" yWindow="3270" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{8BC3A6FB-C4A9-407E-B9A5-41C8CA744755}"/>
+    <workbookView xWindow="7200" yWindow="3270" windowWidth="21600" windowHeight="11295" xr2:uid="{8BC3A6FB-C4A9-407E-B9A5-41C8CA744755}"/>
   </bookViews>
   <sheets>
     <sheet name="Regras-de-Negocio" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
   <si>
     <t>RN001</t>
   </si>
@@ -50,39 +50,12 @@
     <t>IDENTIFICADOR:</t>
   </si>
   <si>
-    <t>O plano premium de um usuário poder ter um ou mais registros de pagamentos;</t>
-  </si>
-  <si>
     <t>RN002</t>
   </si>
   <si>
-    <t>Pagamento do plano premium;</t>
-  </si>
-  <si>
     <t>RN003</t>
   </si>
   <si>
-    <t>RN004</t>
-  </si>
-  <si>
-    <t>Plano premium;</t>
-  </si>
-  <si>
-    <t>O plano premium só será aplicado ao perfil do usuário se não houver pagamento pendente;</t>
-  </si>
-  <si>
-    <t>O Usuário para poder acessar as funções relacionadas as suas metas, além da função incluir, deve ter incluida em seu perfil no mínimo uma meta das disponíveis no sistema;</t>
-  </si>
-  <si>
-    <t>Funções de metas do usuário;</t>
-  </si>
-  <si>
-    <t>Progressão das metas;</t>
-  </si>
-  <si>
-    <t>Para que as progressões de metas sejam acompanhadas pelo usuário, o mesmo deve efetuar registros de acordo com a periodicidade de preenchimento estabelecida para aquela meta;</t>
-  </si>
-  <si>
     <t>REGRAS DE NEGÓCIO (RN)</t>
   </si>
   <si>
@@ -98,15 +71,6 @@
     <t>Cadastrar Usuario;</t>
   </si>
   <si>
-    <t>Adquirir conta premium;</t>
-  </si>
-  <si>
-    <t>Cadastrar cartão de credito;</t>
-  </si>
-  <si>
-    <t>Validar pagamento da assinatura;</t>
-  </si>
-  <si>
     <t>Incluir metas para si;</t>
   </si>
   <si>
@@ -137,10 +101,31 @@
     <t>RF007</t>
   </si>
   <si>
+    <t>Metas do usuário;</t>
+  </si>
+  <si>
+    <t>Usuário;</t>
+  </si>
+  <si>
+    <t>Cada úsuario terá uma conta atrelada a um perfil de condicionamentos iniciais;</t>
+  </si>
+  <si>
+    <t>O usuário deverá ter no mínimo uma meta atribuida para sí;</t>
+  </si>
+  <si>
+    <t>O usuário deve efetuar registros de acordo com a periodicidade de preenchimento estabelecida para cada meta por ele estabelecida;</t>
+  </si>
+  <si>
+    <t>Acompanhamentos das metas;</t>
+  </si>
+  <si>
     <t>RF008</t>
   </si>
   <si>
-    <t>RF009</t>
+    <t>Acompanhar progressão de metas;</t>
+  </si>
+  <si>
+    <t>Login e Logout no aplicativo;</t>
   </si>
 </sst>
 </file>
@@ -541,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{969B9835-71EB-4CCD-B964-F2EBE77482DF}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="45" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -554,7 +539,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B1" s="6"/>
     </row>
@@ -572,7 +557,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -580,7 +565,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -589,7 +574,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -597,7 +582,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -605,7 +590,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -614,7 +599,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -622,7 +607,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -630,7 +615,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -638,25 +623,19 @@
       <c r="A15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -688,10 +667,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08F0151-D227-4A4D-A94B-6AAA158197DD}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="45" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -702,7 +681,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B1" s="6"/>
     </row>
@@ -712,7 +691,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -720,7 +699,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -729,7 +708,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -737,7 +716,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -746,7 +725,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -754,7 +733,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -763,7 +742,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -771,7 +750,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -780,7 +759,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -788,7 +767,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -797,7 +776,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -805,7 +784,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -814,7 +793,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -822,7 +801,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -831,7 +810,7 @@
         <v>3</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -839,24 +818,7 @@
         <v>2</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>